<commit_message>
structure + rewrite of model class
</commit_message>
<xml_diff>
--- a/test_spreadsheet.xlsx
+++ b/test_spreadsheet.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="77">
-  <si>
-    <t xml:space="preserve">Project ID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
+  <si>
+    <t xml:space="preserve">Project</t>
   </si>
   <si>
     <t xml:space="preserve">Owner</t>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Format</t>
   </si>
   <si>
-    <t xml:space="preserve">Notes</t>
+    <t xml:space="preserve">comments</t>
   </si>
   <si>
     <t xml:space="preserve">VAA0000</t>
@@ -151,6 +151,9 @@
     <t xml:space="preserve">Fire in Babylon</t>
   </si>
   <si>
+    <t xml:space="preserve">umatic</t>
+  </si>
+  <si>
     <t xml:space="preserve">VAA0008</t>
   </si>
   <si>
@@ -175,6 +178,9 @@
     <t xml:space="preserve">That Bastard Race</t>
   </si>
   <si>
+    <t xml:space="preserve">open_reel_audio</t>
+  </si>
+  <si>
     <t xml:space="preserve">VAA0010</t>
   </si>
   <si>
@@ -244,13 +250,10 @@
     <t xml:space="preserve">second volume</t>
   </si>
   <si>
-    <t xml:space="preserve">lp</t>
-  </si>
-  <si>
     <t xml:space="preserve">third volume</t>
   </si>
   <si>
-    <t xml:space="preserve">vhs</t>
+    <t xml:space="preserve">fourth volume</t>
   </si>
 </sst>
 </file>
@@ -361,7 +364,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -403,6 +406,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -529,10 +536,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -540,7 +547,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="102.02"/>
   </cols>
@@ -725,25 +732,25 @@
         <v>42</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="I8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>16</v>
@@ -752,40 +759,40 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>16</v>
@@ -794,138 +801,149 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F12" s="9" t="n">
         <v>40000003619386</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F13" s="9" t="n">
         <v>40000003619378</v>
       </c>
       <c r="G13" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F14" s="9" t="n">
         <v>40000003619352</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F15" s="9" t="n">
         <v>40000003619360</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F17" s="1" t="n">
-        <v>40000003841234</v>
+        <v>40000003841238</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F18" s="1" t="n">
-        <v>40000003841235</v>
+        <v>40000003841246</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F19" s="1" t="n">
-        <v>40000003841236</v>
+        <v>40000003841253</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>76</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F20" s="1" t="n">
+        <v>40000003841261</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>